<commit_message>
Commencement du java / faire les classes
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065CC0DC-8CA3-458A-8AD1-2DDC1156A4D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683C47DF-0AEF-4B9A-BCB9-9BFC5E2997B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve">Salut je suis arthur et je suis un gros con </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">id du client : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">id du chauffeur : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">heure de début : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heure de fin : </t>
+  </si>
+  <si>
+    <t>dateReservation :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance du trajet : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix du trajet : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieu de début : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieu de fin : </t>
+  </si>
+  <si>
+    <t>Durée du trajet :</t>
+  </si>
+  <si>
+    <t>id du trajet :</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Marseille</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>Bordeaux</t>
   </si>
 </sst>
 </file>
@@ -58,8 +100,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,15 +384,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.42372685185185183</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.43078703703703702</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43862</v>
+      </c>
+      <c r="G2">
+        <v>120</v>
+      </c>
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.84733796296296304</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.93078703703703702</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43648</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3">
+        <v>230</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push excel ajout bdd
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9831EBF5-7094-4965-82D6-03986BC2938A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD8A780-48F9-4041-96D4-AB7B48C1E837}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">id du client : </t>
   </si>
@@ -52,9 +52,6 @@
     <t>Durée du trajet :</t>
   </si>
   <si>
-    <t>id du trajet :</t>
-  </si>
-  <si>
     <t>Paris</t>
   </si>
   <si>
@@ -65,6 +62,15 @@
   </si>
   <si>
     <t>Bordeaux</t>
+  </si>
+  <si>
+    <t>Montpellier</t>
+  </si>
+  <si>
+    <t>Id du trajet</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -386,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" style="1" customWidth="1"/>
@@ -409,7 +415,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -443,6 +449,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12</v>
+      </c>
       <c r="B2">
         <v>22</v>
       </c>
@@ -465,16 +474,19 @@
         <v>1000</v>
       </c>
       <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
       </c>
       <c r="K2">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
       <c r="B3">
         <v>21</v>
       </c>
@@ -497,13 +509,48 @@
         <v>230</v>
       </c>
       <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
       </c>
       <c r="K3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44114.416666666664</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44114.416666666664</v>
+      </c>
+      <c r="F4" s="1">
+        <v>43545.635775462964</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>2000</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>